<commit_message>
2016/08/19  Changes to be committed: 	modified:   overtime.xlsx
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:P156"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1073,24 +1073,24 @@
         <v>42583</v>
       </c>
       <c r="B13">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C13">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.78333333333333333</v>
+        <v>0.68333333333333335</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>0.6166666666666667</v>
+        <v>0.78333333333333333</v>
       </c>
       <c r="H13">
         <v>9</v>
@@ -1104,18 +1104,18 @@
       </c>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
-        <v>29.783333333333335</v>
+        <v>36.68333333333333</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="5"/>
-        <v>195.51666666666668</v>
+        <v>202.41666666666669</v>
       </c>
       <c r="M13">
         <v>1370</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="4"/>
-        <v>54267.983333333344</v>
+        <v>66956.466666666674</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>195.51666666666668</v>
+        <v>202.41666666666669</v>
       </c>
       <c r="M14">
         <v>1370</v>
@@ -1159,7 +1159,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>343855.2</v>
+        <v>356543.68333333335</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
2016/08/30 modified module garage in train
 Changes to be committed:
	modified:   mypro/C#/train/train.v11.suo
	modified:   mypro/C#/train/train/App.config
	modified:   mypro/C#/train/train/CSV.cs
	modified:   mypro/C#/train/train/Form1.cs
	modified:   mypro/C#/train/train/Parameter.cs
	modified:   mypro/C#/train/train/Properties/Settings.Designer.cs
	modified:   mypro/C#/train/train/Properties/Settings.settings
	copied:     mypro/C#/train/train/App.config -> mypro/C#/train/train/bin/Debug/train.exe.config
	modified:   mypro/C#/train/train/bin/Debug/train.vshost.exe.config
	modified:   overtime.xlsx
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:P157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1073,14 +1073,14 @@
         <v>42583</v>
       </c>
       <c r="B13">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
-        <v>0.35</v>
+        <v>0.96666666666666667</v>
       </c>
       <c r="E13">
         <v>2</v>
@@ -1104,18 +1104,18 @@
       </c>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
-        <v>44.35</v>
+        <v>51.966666666666669</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="5"/>
-        <v>210.08333333333334</v>
+        <v>217.70000000000002</v>
       </c>
       <c r="M13">
         <v>1370</v>
       </c>
       <c r="N13" s="6">
         <f t="shared" si="4"/>
-        <v>80610.800000000017</v>
+        <v>94176.083333333358</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.15">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>210.08333333333334</v>
+        <v>217.70000000000002</v>
       </c>
       <c r="M14">
         <v>1370</v>
@@ -1159,7 +1159,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>370198.01666666672</v>
+        <v>383763.30000000005</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Initialization module(100%)  Changes between modules(20%)
 Changes to be committed:
	modified:   mypro/C#/train/train.v11.suo
	modified:   mypro/C#/train/train/CSV.cs
	modified:   mypro/C#/train/train/Form1.Designer.cs
	modified:   mypro/C#/train/train/Form1.cs
	modified:   mypro/C#/train/train/bin/Debug/Record/custom.csv
	modified:   mypro/C#/train/train/bin/Debug/train.exe
	modified:   mypro/C#/train/train/bin/Debug/train.pdb
	modified:   mypro/C#/train/train/obj/Debug/DesignTimeResolveAssemblyReferencesInput.cache
	modified:   mypro/C#/train/train/obj/Debug/train.csproj.GenerateResource.Cache
	modified:   mypro/C#/train/train/obj/Debug/train.exe
	modified:   mypro/C#/train/train/obj/Debug/train.pdb
	modified:   overtime.xlsx
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="165" windowWidth="28035" windowHeight="12060"/>
+    <workbookView xWindow="360" yWindow="180" windowWidth="28035" windowHeight="12045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:P157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1122,9 +1122,15 @@
       <c r="A14" s="3">
         <v>42614</v>
       </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>25</v>
+      </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -1136,18 +1142,18 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.4166666666666667</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>222.45000000000002</v>
+        <v>223.86666666666667</v>
       </c>
       <c r="M14">
         <v>1370</v>
       </c>
       <c r="N14" s="6">
         <f>K14*M14*1.3+(E14+G14)*M14*0.25+(H14+J14)*M14*0.05</f>
-        <v>0</v>
+        <v>2523.0833333333335</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -1159,7 +1165,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>392223.05000000005</v>
+        <v>394746.13333333336</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
9/9 Form optimization 30%
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="180" windowWidth="28035" windowHeight="12045"/>
+    <workbookView xWindow="360" yWindow="195" windowWidth="28035" windowHeight="12030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
   <dimension ref="A1:P157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1123,14 +1123,14 @@
         <v>42614</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C14">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.11666666666666667</v>
+        <v>0.7</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -1142,18 +1142,18 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>6.1166666666666663</v>
+        <v>7.7</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>228.56666666666669</v>
+        <v>230.15</v>
       </c>
       <c r="M14">
         <v>1370</v>
       </c>
       <c r="N14" s="6">
         <f>K14*M14*1.3+(E14+G14)*M14*0.25+(H14+J14)*M14*0.05</f>
-        <v>10893.783333333333</v>
+        <v>13713.7</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -1165,7 +1165,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>403116.83333333337</v>
+        <v>405936.75000000006</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
As a result of Google Maps, the game was redesigned
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -498,7 +498,7 @@
   <dimension ref="A1:P157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1123,14 +1123,14 @@
         <v>42614</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -1142,18 +1142,18 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>11.05</v>
+        <v>13.833333333333334</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>233.50000000000003</v>
+        <v>236.28333333333336</v>
       </c>
       <c r="M14">
         <v>1370</v>
       </c>
       <c r="N14" s="6">
         <f>K14*M14*1.3+(E14+G14)*M14*0.25+(H14+J14)*M14*0.05</f>
-        <v>19680.050000000003</v>
+        <v>24637.166666666668</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -1165,7 +1165,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>411903.10000000003</v>
+        <v>416860.21666666673</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
Add city Manage module (20%)
</commit_message>
<xml_diff>
--- a/overtime.xlsx
+++ b/overtime.xlsx
@@ -1123,14 +1123,14 @@
         <v>42614</v>
       </c>
       <c r="B14">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
-        <v>0.83333333333333337</v>
+        <v>0.68333333333333335</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
@@ -1142,18 +1142,18 @@
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
-        <v>13.833333333333334</v>
+        <v>18.683333333333334</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
-        <v>236.28333333333336</v>
+        <v>241.13333333333335</v>
       </c>
       <c r="M14">
         <v>1370</v>
       </c>
       <c r="N14" s="6">
         <f>K14*M14*1.3+(E14+G14)*M14*0.25+(H14+J14)*M14*0.05</f>
-        <v>24637.166666666668</v>
+        <v>33275.01666666667</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.15">
@@ -1165,7 +1165,7 @@
       <c r="L15" s="1"/>
       <c r="N15" s="6">
         <f>SUM(N3:N14)</f>
-        <v>416860.21666666673</v>
+        <v>425498.06666666671</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.15">

</xml_diff>